<commit_message>
add generated tptp files
</commit_message>
<xml_diff>
--- a/2020-FASE/FASE2020-GlobalData.xlsx
+++ b/2020-FASE/FASE2020-GlobalData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/aren_babikian_mail_mcgill_ca/Documents/FASE 2020/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aren Babikian\git\publication-pages\2020-FASE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="435" documentId="13_ncr:1_{04545327-DB47-4D6B-9EC8-5C1B031BC182}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E96467BA-3B08-47FD-9785-1D3481229752}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61AB01E7-6A09-4308-B68E-7B609D7695DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="759" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="759" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CVC4" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -11244,15 +11246,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>21869</xdr:rowOff>
+      <xdr:colOff>183173</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>124446</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>273823</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>137443</xdr:rowOff>
+      <xdr:colOff>266496</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>49520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11316,15 +11318,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>207848</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>179128</xdr:rowOff>
+      <xdr:colOff>222502</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>98532</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>345939</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>189806</xdr:rowOff>
+      <xdr:colOff>360593</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>109210</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11352,15 +11354,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>246590</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>27331</xdr:rowOff>
+      <xdr:colOff>158667</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>107927</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>184005</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>190139</xdr:rowOff>
+      <xdr:colOff>96082</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>80235</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -52530,7 +52532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7143E68-3C99-495D-AC26-75A25E956AD4}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>

</xml_diff>